<commit_message>
update video description & comment compare uploaded and listed videos remove draft videos
</commit_message>
<xml_diff>
--- a/input/videos_prod.xlsx
+++ b/input/videos_prod.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3309" uniqueCount="1332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3234" uniqueCount="1294">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -3886,120 +3886,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/GmXWs6dHS3c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Udvar területe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/admin/exercise/edit/-MM7x5KFmyGweMBTjUtD#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/exercise/-MM7x5KFmyGweMBTjUtD#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometria 46. Téglalap területe - SZÖVEGES FELADAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=dBULZRj2V1g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UgzbRfGh5uJxWP4rtuV4AaABAg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 téglalap területe kerülete szöveges feladat.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Termőföld területe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/admin/exercise/edit/-MM9MT2O9uEyVgG-LWO8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/exercise/-MM9MT2O9uEyVgG-LWO8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometria 47. Téglalap területe arányokkal - SZÖVEGES FELADAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=WgQRJfxovAc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ugwj2gyDhlWrOaD3f3F4AaABAg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 téglalap területe szöveges feladat.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubik kocka felszíne, térfogata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/admin/exercise/edit/-MM9QrnKdYBDIku7us0W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/exercise/-MM9QrnKdYBDIku7us0W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometria 48. Rubik torony felszíne, térfogata - SZÖVEGES FELADAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=V-V0l1y9FA4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UgzHuk-OWWnFFGJnTep4AaABAg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 téglatest térfogata felszíne rubik kocka szöveges feladat.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lapátló, testátló</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/admin/exercise/edit/-MM9Y3txq5LDMLd5pfaP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/exercise/-MM9Y3txq5LDMLd5pfaP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometria 49. Testek lapátlója, testátlója</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=Of0mM7_lD-c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ugy9vaPM7umpvINLlBh4AaABAg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. osztály,lapátló jelentése,síkidom jelentése,síkidomok 5 osztály,síkidomok átlóinak száma,síkidomok sokszögek 5. osztály,sokszög átló számítás,sokszög átlóinak száma,sokszög fogalma,sokszög összes átlója,sokszögek fajtái,sokszögek tulajdonságai,testátló fogalma,testátló jelentése</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 geometria lapátló testátló.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logikai fejtörő</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Einstein feladványa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/admin/exercise/edit/-MM9cPoK1c2JB0roRmnh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://zsebtanar.hu/exercise/-MM9cPoK1c2JB0roRmnh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Einstein feladványa – Te meg tudod oldani?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=sd6hCb8ezXY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UgynWRWrfIdg_MkWUD14AaABAg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Einstein feladványa, logikai feladat, brit, német, dán, svéd, Einstein fejtörő, IQ, két százalék</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 logikai feladvány einstein.mp4</t>
   </si>
   <si>
     <t xml:space="preserve">PlaylistOrder</t>
@@ -4303,14 +4189,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ163"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H148" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A148" activeCellId="0" sqref="A148"/>
-      <selection pane="bottomRight" activeCell="N163" activeCellId="0" sqref="N163"/>
+      <selection pane="bottomRight" activeCell="A159" activeCellId="0" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13454,256 +13340,11 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="n">
-        <v>158</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>1054</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>1278</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>1279</v>
-      </c>
-      <c r="G159" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="I159" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="J159" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K159" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L159" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M159" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O159" s="1" t="s">
-        <v>1282</v>
-      </c>
-      <c r="P159" s="1" t="s">
-        <v>1283</v>
-      </c>
-      <c r="Q159" s="1" t="s">
-        <v>1062</v>
-      </c>
-      <c r="R159" s="1" t="s">
-        <v>1284</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="n">
-        <v>159</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>1054</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>1286</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>1287</v>
-      </c>
-      <c r="I160" s="1" t="s">
-        <v>1288</v>
-      </c>
-      <c r="J160" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K160" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L160" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M160" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O160" s="1" t="s">
-        <v>1289</v>
-      </c>
-      <c r="P160" s="1" t="s">
-        <v>1290</v>
-      </c>
-      <c r="Q160" s="1" t="s">
-        <v>1062</v>
-      </c>
-      <c r="R160" s="1" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="n">
-        <v>160</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>1292</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>1293</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>1294</v>
-      </c>
-      <c r="I161" s="1" t="s">
-        <v>1295</v>
-      </c>
-      <c r="J161" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K161" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L161" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M161" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O161" s="1" t="s">
-        <v>1296</v>
-      </c>
-      <c r="P161" s="1" t="s">
-        <v>1297</v>
-      </c>
-      <c r="Q161" s="1" t="s">
-        <v>1126</v>
-      </c>
-      <c r="R161" s="1" t="s">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="n">
-        <v>161</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>887</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>1299</v>
-      </c>
-      <c r="F162" s="1" t="s">
-        <v>1300</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>1301</v>
-      </c>
-      <c r="I162" s="1" t="s">
-        <v>1302</v>
-      </c>
-      <c r="J162" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K162" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L162" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M162" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O162" s="1" t="s">
-        <v>1303</v>
-      </c>
-      <c r="P162" s="1" t="s">
-        <v>1304</v>
-      </c>
-      <c r="Q162" s="1" t="s">
-        <v>1305</v>
-      </c>
-      <c r="R162" s="1" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="n">
-        <v>162</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>1307</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>1308</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>1309</v>
-      </c>
-      <c r="G163" s="1" t="s">
-        <v>1310</v>
-      </c>
-      <c r="I163" s="1" t="s">
-        <v>1311</v>
-      </c>
-      <c r="J163" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K163" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L163" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M163" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O163" s="1" t="s">
-        <v>1312</v>
-      </c>
-      <c r="P163" s="1" t="s">
-        <v>1313</v>
-      </c>
-      <c r="Q163" s="1" t="s">
-        <v>1314</v>
-      </c>
-      <c r="R163" s="1" t="s">
-        <v>1315</v>
-      </c>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -13744,10 +13385,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>1316</v>
+        <v>1278</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>1317</v>
+        <v>1279</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
@@ -13756,13 +13397,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>1318</v>
+        <v>1280</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>1319</v>
+        <v>1281</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>1320</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13770,7 +13411,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1321</v>
+        <v>1283</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
@@ -13794,7 +13435,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1321</v>
+        <v>1283</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -13818,7 +13459,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1321</v>
+        <v>1283</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
@@ -13842,7 +13483,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1321</v>
+        <v>1283</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
@@ -13866,7 +13507,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1321</v>
+        <v>1283</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>19</v>
@@ -13890,7 +13531,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1321</v>
+        <v>1283</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -13914,7 +13555,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1322</v>
+        <v>1284</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -13938,7 +13579,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1322</v>
+        <v>1284</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
@@ -13962,7 +13603,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1322</v>
+        <v>1284</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>
@@ -13986,7 +13627,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1322</v>
+        <v>1284</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
@@ -14010,7 +13651,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1322</v>
+        <v>1284</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>19</v>
@@ -14034,7 +13675,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1322</v>
+        <v>1284</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>19</v>
@@ -14058,7 +13699,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1323</v>
+        <v>1285</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>19</v>
@@ -14082,7 +13723,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1323</v>
+        <v>1285</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
@@ -14106,7 +13747,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1323</v>
+        <v>1285</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>19</v>
@@ -14130,7 +13771,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1323</v>
+        <v>1285</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
@@ -14154,7 +13795,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>19</v>
@@ -14178,7 +13819,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>19</v>
@@ -14202,7 +13843,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>19</v>
@@ -14226,7 +13867,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>19</v>
@@ -14250,7 +13891,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>19</v>
@@ -14274,7 +13915,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>19</v>
@@ -14298,7 +13939,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>19</v>
@@ -14322,7 +13963,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>19</v>
@@ -14346,7 +13987,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>19</v>
@@ -14370,7 +14011,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>19</v>
@@ -14394,7 +14035,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>19</v>
@@ -14418,7 +14059,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>19</v>
@@ -14442,7 +14083,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>19</v>
@@ -14466,7 +14107,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>19</v>
@@ -14490,7 +14131,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>19</v>
@@ -14514,7 +14155,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>19</v>
@@ -14538,7 +14179,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>19</v>
@@ -14562,7 +14203,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>19</v>
@@ -14586,7 +14227,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>19</v>
@@ -14610,7 +14251,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>19</v>
@@ -14634,7 +14275,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>19</v>
@@ -14658,7 +14299,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>19</v>
@@ -14682,7 +14323,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>19</v>
@@ -14706,7 +14347,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>19</v>
@@ -14730,7 +14371,7 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>19</v>
@@ -14754,7 +14395,7 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>19</v>
@@ -14778,7 +14419,7 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1324</v>
+        <v>1286</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>19</v>
@@ -14802,7 +14443,7 @@
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>19</v>
@@ -14826,7 +14467,7 @@
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>19</v>
@@ -14850,7 +14491,7 @@
         <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>19</v>
@@ -14874,7 +14515,7 @@
         <v>5</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>19</v>
@@ -14898,7 +14539,7 @@
         <v>5</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>19</v>
@@ -14922,7 +14563,7 @@
         <v>5</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>19</v>
@@ -14946,7 +14587,7 @@
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>19</v>
@@ -14970,7 +14611,7 @@
         <v>5</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>19</v>
@@ -14994,7 +14635,7 @@
         <v>5</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>19</v>
@@ -15018,7 +14659,7 @@
         <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>19</v>
@@ -15042,7 +14683,7 @@
         <v>5</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>19</v>
@@ -15066,7 +14707,7 @@
         <v>5</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>19</v>
@@ -15090,7 +14731,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>19</v>
@@ -15114,7 +14755,7 @@
         <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>19</v>
@@ -15138,7 +14779,7 @@
         <v>5</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>19</v>
@@ -15162,7 +14803,7 @@
         <v>5</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>19</v>
@@ -15186,7 +14827,7 @@
         <v>5</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>19</v>
@@ -15210,7 +14851,7 @@
         <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>19</v>
@@ -15234,7 +14875,7 @@
         <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>19</v>
@@ -15258,7 +14899,7 @@
         <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>19</v>
@@ -15282,7 +14923,7 @@
         <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>19</v>
@@ -15306,7 +14947,7 @@
         <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>19</v>
@@ -15330,7 +14971,7 @@
         <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>19</v>
@@ -15354,7 +14995,7 @@
         <v>5</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>19</v>
@@ -15378,7 +15019,7 @@
         <v>5</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>19</v>
@@ -15402,7 +15043,7 @@
         <v>5</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>19</v>
@@ -15426,7 +15067,7 @@
         <v>5</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>19</v>
@@ -15450,7 +15091,7 @@
         <v>5</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>19</v>
@@ -15474,7 +15115,7 @@
         <v>5</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>19</v>
@@ -15498,7 +15139,7 @@
         <v>5</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>19</v>
@@ -15522,7 +15163,7 @@
         <v>5</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>19</v>
@@ -15546,7 +15187,7 @@
         <v>5</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>19</v>
@@ -15570,7 +15211,7 @@
         <v>5</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>19</v>
@@ -15594,7 +15235,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>19</v>
@@ -15618,7 +15259,7 @@
         <v>5</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>19</v>
@@ -15642,7 +15283,7 @@
         <v>5</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1325</v>
+        <v>1287</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>19</v>
@@ -15666,7 +15307,7 @@
         <v>6</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>19</v>
@@ -15690,7 +15331,7 @@
         <v>6</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>19</v>
@@ -15714,7 +15355,7 @@
         <v>6</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>19</v>
@@ -15738,7 +15379,7 @@
         <v>6</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>19</v>
@@ -15762,7 +15403,7 @@
         <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>19</v>
@@ -15786,7 +15427,7 @@
         <v>6</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>19</v>
@@ -15810,7 +15451,7 @@
         <v>6</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>19</v>
@@ -15834,7 +15475,7 @@
         <v>6</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>19</v>
@@ -15858,7 +15499,7 @@
         <v>6</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>19</v>
@@ -15882,7 +15523,7 @@
         <v>6</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>19</v>
@@ -15906,7 +15547,7 @@
         <v>6</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>19</v>
@@ -15930,7 +15571,7 @@
         <v>6</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>19</v>
@@ -15954,7 +15595,7 @@
         <v>6</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>19</v>
@@ -15978,7 +15619,7 @@
         <v>6</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>19</v>
@@ -16002,7 +15643,7 @@
         <v>6</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>1326</v>
+        <v>1288</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>19</v>
@@ -16026,7 +15667,7 @@
         <v>7</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>19</v>
@@ -16050,7 +15691,7 @@
         <v>7</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>19</v>
@@ -16074,7 +15715,7 @@
         <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>19</v>
@@ -16098,7 +15739,7 @@
         <v>7</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>19</v>
@@ -16122,7 +15763,7 @@
         <v>7</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>19</v>
@@ -16146,7 +15787,7 @@
         <v>7</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>19</v>
@@ -16170,7 +15811,7 @@
         <v>7</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>19</v>
@@ -16194,7 +15835,7 @@
         <v>7</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>19</v>
@@ -16218,7 +15859,7 @@
         <v>7</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>19</v>
@@ -16242,7 +15883,7 @@
         <v>7</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>19</v>
@@ -16266,7 +15907,7 @@
         <v>7</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1327</v>
+        <v>1289</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>19</v>
@@ -16290,7 +15931,7 @@
         <v>8</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>19</v>
@@ -16314,7 +15955,7 @@
         <v>8</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>19</v>
@@ -16338,7 +15979,7 @@
         <v>8</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>19</v>
@@ -16362,7 +16003,7 @@
         <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>19</v>
@@ -16386,7 +16027,7 @@
         <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>19</v>
@@ -16410,7 +16051,7 @@
         <v>8</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>19</v>
@@ -16434,7 +16075,7 @@
         <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>19</v>
@@ -16458,7 +16099,7 @@
         <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>19</v>
@@ -16482,7 +16123,7 @@
         <v>8</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>19</v>
@@ -16506,7 +16147,7 @@
         <v>8</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>19</v>
@@ -16530,7 +16171,7 @@
         <v>8</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>19</v>
@@ -16554,7 +16195,7 @@
         <v>8</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>19</v>
@@ -16578,7 +16219,7 @@
         <v>8</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>19</v>
@@ -16602,7 +16243,7 @@
         <v>8</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>19</v>
@@ -16626,7 +16267,7 @@
         <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>19</v>
@@ -16650,7 +16291,7 @@
         <v>8</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>19</v>
@@ -16674,7 +16315,7 @@
         <v>8</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>19</v>
@@ -16698,7 +16339,7 @@
         <v>8</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>19</v>
@@ -16722,7 +16363,7 @@
         <v>8</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>19</v>
@@ -16746,7 +16387,7 @@
         <v>8</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>19</v>
@@ -16770,7 +16411,7 @@
         <v>8</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>19</v>
@@ -16794,7 +16435,7 @@
         <v>8</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>19</v>
@@ -16818,7 +16459,7 @@
         <v>8</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>19</v>
@@ -16842,7 +16483,7 @@
         <v>8</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>19</v>
@@ -16866,7 +16507,7 @@
         <v>8</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>19</v>
@@ -16890,7 +16531,7 @@
         <v>8</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>19</v>
@@ -16914,7 +16555,7 @@
         <v>8</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>19</v>
@@ -16938,7 +16579,7 @@
         <v>8</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>19</v>
@@ -16962,7 +16603,7 @@
         <v>8</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>19</v>
@@ -16986,7 +16627,7 @@
         <v>8</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>19</v>
@@ -17010,7 +16651,7 @@
         <v>8</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>19</v>
@@ -17034,7 +16675,7 @@
         <v>8</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>19</v>
@@ -17058,7 +16699,7 @@
         <v>8</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>19</v>
@@ -17082,7 +16723,7 @@
         <v>8</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>19</v>
@@ -17106,7 +16747,7 @@
         <v>8</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>19</v>
@@ -17130,7 +16771,7 @@
         <v>8</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>19</v>
@@ -17154,7 +16795,7 @@
         <v>8</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>19</v>
@@ -17178,7 +16819,7 @@
         <v>8</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>19</v>
@@ -17202,7 +16843,7 @@
         <v>8</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>19</v>
@@ -17226,7 +16867,7 @@
         <v>8</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>19</v>
@@ -17250,7 +16891,7 @@
         <v>8</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>19</v>
@@ -17274,7 +16915,7 @@
         <v>8</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>19</v>
@@ -17298,7 +16939,7 @@
         <v>8</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>19</v>
@@ -17322,7 +16963,7 @@
         <v>8</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>19</v>
@@ -17346,7 +16987,7 @@
         <v>8</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>19</v>
@@ -17370,7 +17011,7 @@
         <v>8</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>19</v>
@@ -17386,7 +17027,7 @@
       </c>
       <c r="G152" s="10" t="str">
         <f aca="false">IFERROR(VLOOKUP(F152,Videos!A:I,9,FALSE()),"")</f>
-        <v>Geometria 46. Téglalap területe - SZÖVEGES FELADAT</v>
+        <v/>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17394,7 +17035,7 @@
         <v>8</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>19</v>
@@ -17410,7 +17051,7 @@
       </c>
       <c r="G153" s="10" t="str">
         <f aca="false">IFERROR(VLOOKUP(F153,Videos!A:I,9,FALSE()),"")</f>
-        <v>Geometria 47. Téglalap területe arányokkal - SZÖVEGES FELADAT</v>
+        <v/>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17418,7 +17059,7 @@
         <v>8</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>19</v>
@@ -17434,7 +17075,7 @@
       </c>
       <c r="G154" s="10" t="str">
         <f aca="false">IFERROR(VLOOKUP(F154,Videos!A:I,9,FALSE()),"")</f>
-        <v>Geometria 48. Rubik torony felszíne, térfogata - SZÖVEGES FELADAT</v>
+        <v/>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17442,7 +17083,7 @@
         <v>8</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>1328</v>
+        <v>1290</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>19</v>
@@ -17458,7 +17099,7 @@
       </c>
       <c r="G155" s="10" t="str">
         <f aca="false">IFERROR(VLOOKUP(F155,Videos!A:I,9,FALSE()),"")</f>
-        <v>Geometria 49. Testek lapátlója, testátlója</v>
+        <v/>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17466,7 +17107,7 @@
         <v>9</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>1329</v>
+        <v>1291</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>19</v>
@@ -17490,7 +17131,7 @@
         <v>9</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>1329</v>
+        <v>1291</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>19</v>
@@ -17514,7 +17155,7 @@
         <v>9</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1329</v>
+        <v>1291</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>19</v>
@@ -17538,7 +17179,7 @@
         <v>9</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1329</v>
+        <v>1291</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>19</v>
@@ -17562,7 +17203,7 @@
         <v>9</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>1329</v>
+        <v>1291</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>19</v>
@@ -17586,7 +17227,7 @@
         <v>9</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>1329</v>
+        <v>1291</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>19</v>
@@ -17610,7 +17251,7 @@
         <v>10</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>19</v>
@@ -17634,7 +17275,7 @@
         <v>10</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>19</v>
@@ -17658,7 +17299,7 @@
         <v>10</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>19</v>
@@ -17682,7 +17323,7 @@
         <v>10</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>19</v>
@@ -17706,7 +17347,7 @@
         <v>10</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>19</v>
@@ -17730,7 +17371,7 @@
         <v>10</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>19</v>
@@ -17754,7 +17395,7 @@
         <v>10</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>19</v>
@@ -17778,7 +17419,7 @@
         <v>10</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>19</v>
@@ -17802,7 +17443,7 @@
         <v>10</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>19</v>
@@ -17826,7 +17467,7 @@
         <v>10</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>19</v>
@@ -17850,7 +17491,7 @@
         <v>10</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>19</v>
@@ -17874,7 +17515,7 @@
         <v>10</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>19</v>
@@ -17898,7 +17539,7 @@
         <v>10</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>19</v>
@@ -17922,7 +17563,7 @@
         <v>10</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>19</v>
@@ -17946,7 +17587,7 @@
         <v>10</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>19</v>
@@ -17970,7 +17611,7 @@
         <v>10</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>19</v>
@@ -17994,7 +17635,7 @@
         <v>10</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>19</v>
@@ -18018,7 +17659,7 @@
         <v>10</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>19</v>
@@ -18042,7 +17683,7 @@
         <v>10</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>19</v>
@@ -18066,7 +17707,7 @@
         <v>10</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>19</v>
@@ -18090,7 +17731,7 @@
         <v>10</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>19</v>
@@ -18114,7 +17755,7 @@
         <v>10</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>19</v>
@@ -18138,7 +17779,7 @@
         <v>10</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>19</v>
@@ -18162,7 +17803,7 @@
         <v>10</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>19</v>
@@ -18186,7 +17827,7 @@
         <v>10</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>19</v>
@@ -18210,7 +17851,7 @@
         <v>10</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>19</v>
@@ -18234,7 +17875,7 @@
         <v>10</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>19</v>
@@ -18258,7 +17899,7 @@
         <v>10</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>19</v>
@@ -18282,7 +17923,7 @@
         <v>10</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>19</v>
@@ -18306,7 +17947,7 @@
         <v>10</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>19</v>
@@ -18330,7 +17971,7 @@
         <v>10</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>19</v>
@@ -18354,7 +17995,7 @@
         <v>10</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>19</v>
@@ -18378,7 +18019,7 @@
         <v>10</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>19</v>
@@ -18402,7 +18043,7 @@
         <v>10</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>19</v>
@@ -18426,7 +18067,7 @@
         <v>10</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>19</v>
@@ -18450,7 +18091,7 @@
         <v>10</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>19</v>
@@ -18474,7 +18115,7 @@
         <v>10</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>19</v>
@@ -18498,7 +18139,7 @@
         <v>10</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>19</v>
@@ -18522,7 +18163,7 @@
         <v>10</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>19</v>
@@ -18546,7 +18187,7 @@
         <v>10</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>19</v>
@@ -18570,7 +18211,7 @@
         <v>10</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>19</v>
@@ -18594,7 +18235,7 @@
         <v>10</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>19</v>
@@ -18618,7 +18259,7 @@
         <v>10</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>19</v>
@@ -18642,7 +18283,7 @@
         <v>10</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>1330</v>
+        <v>1292</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>19</v>
@@ -18666,7 +18307,7 @@
         <v>11</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>19</v>
@@ -18690,7 +18331,7 @@
         <v>11</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>19</v>
@@ -18714,7 +18355,7 @@
         <v>11</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>19</v>
@@ -18738,7 +18379,7 @@
         <v>11</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>19</v>
@@ -18762,7 +18403,7 @@
         <v>11</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>19</v>
@@ -18786,7 +18427,7 @@
         <v>11</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>19</v>
@@ -18810,7 +18451,7 @@
         <v>11</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>19</v>
@@ -18834,7 +18475,7 @@
         <v>11</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>19</v>
@@ -18858,7 +18499,7 @@
         <v>11</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>19</v>
@@ -18882,7 +18523,7 @@
         <v>11</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>19</v>
@@ -18906,7 +18547,7 @@
         <v>11</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>19</v>
@@ -18930,7 +18571,7 @@
         <v>11</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>19</v>
@@ -18954,7 +18595,7 @@
         <v>11</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>1331</v>
+        <v>1293</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>19</v>
@@ -18970,7 +18611,7 @@
       </c>
       <c r="G218" s="10" t="str">
         <f aca="false">IFERROR(VLOOKUP(F218,Videos!A:I,9,FALSE()),"")</f>
-        <v>Einstein feladványa – Te meg tudod oldani?</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>